<commit_message>
flexible colmn names added
</commit_message>
<xml_diff>
--- a/assessment_tree.xlsx
+++ b/assessment_tree.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sharon/GitHub/assessment_tree/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sklinke1/Git Repos/assessment_tree/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="3880" yWindow="440" windowWidth="29220" windowHeight="19440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,12 +398,13 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>